<commit_message>
add mcq pdf file
</commit_message>
<xml_diff>
--- a/Amna Zahid MCQs1.xlsx.xlsx
+++ b/Amna Zahid MCQs1.xlsx.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srmal\Documents\semester6\ead mcqs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00-Intervew-Prepration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0120A8B4-3A3B-47D3-A5DF-5DC6BAA47504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6134,7 +6133,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6597,69 +6596,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -6718,14 +6654,77 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 4" xfId="4" xr:uid="{670B57FA-AE95-4C1D-923D-69FCBD02678C}"/>
-    <cellStyle name="Normal 5" xfId="5" xr:uid="{D636E403-8A6A-42F6-9351-382F037CA21A}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 4" xfId="4"/>
+    <cellStyle name="Normal 5" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7002,11 +7001,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G628"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A433" workbookViewId="0">
-      <selection activeCell="B444" sqref="B444"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8111,145 +8110,145 @@
       </c>
     </row>
     <row r="67" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="78" t="s">
+      <c r="A67" s="80" t="s">
         <v>266</v>
       </c>
-      <c r="B67" s="78"/>
+      <c r="B67" s="80"/>
       <c r="C67" s="14"/>
       <c r="D67" s="14"/>
       <c r="E67" s="2"/>
     </row>
     <row r="68" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="70" t="s">
+      <c r="A68" s="78" t="s">
         <v>267</v>
       </c>
-      <c r="B68" s="70"/>
+      <c r="B68" s="78"/>
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
       <c r="E68" s="2"/>
     </row>
     <row r="69" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="70" t="s">
+      <c r="A69" s="78" t="s">
         <v>268</v>
       </c>
-      <c r="B69" s="70"/>
+      <c r="B69" s="78"/>
       <c r="C69" s="14"/>
       <c r="D69" s="14"/>
       <c r="E69" s="2"/>
     </row>
     <row r="70" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="70" t="s">
+      <c r="A70" s="78" t="s">
         <v>269</v>
       </c>
-      <c r="B70" s="70"/>
+      <c r="B70" s="78"/>
       <c r="C70" s="14"/>
       <c r="D70" s="14"/>
       <c r="E70" s="2"/>
     </row>
     <row r="71" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="77" t="s">
+      <c r="A71" s="79" t="s">
         <v>270</v>
       </c>
-      <c r="B71" s="77"/>
+      <c r="B71" s="79"/>
       <c r="C71" s="14"/>
       <c r="D71" s="14"/>
       <c r="E71" s="2"/>
     </row>
     <row r="72" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="70" t="s">
+      <c r="A72" s="78" t="s">
         <v>271</v>
       </c>
-      <c r="B72" s="70"/>
+      <c r="B72" s="78"/>
       <c r="C72" s="14"/>
       <c r="D72" s="14"/>
       <c r="E72" s="2"/>
     </row>
     <row r="73" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="70" t="s">
+      <c r="A73" s="78" t="s">
         <v>272</v>
       </c>
-      <c r="B73" s="70"/>
+      <c r="B73" s="78"/>
       <c r="C73" s="14"/>
       <c r="D73" s="14"/>
       <c r="E73" s="2"/>
     </row>
     <row r="74" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="70" t="s">
+      <c r="A74" s="78" t="s">
         <v>273</v>
       </c>
-      <c r="B74" s="70"/>
+      <c r="B74" s="78"/>
       <c r="C74" s="14"/>
       <c r="D74" s="14"/>
       <c r="E74" s="2"/>
     </row>
     <row r="75" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="70" t="s">
+      <c r="A75" s="78" t="s">
         <v>274</v>
       </c>
-      <c r="B75" s="70"/>
+      <c r="B75" s="78"/>
       <c r="C75" s="14"/>
       <c r="D75" s="14"/>
       <c r="E75" s="2"/>
     </row>
     <row r="76" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="70" t="s">
+      <c r="A76" s="78" t="s">
         <v>275</v>
       </c>
-      <c r="B76" s="70"/>
+      <c r="B76" s="78"/>
       <c r="C76" s="14"/>
       <c r="D76" s="14"/>
       <c r="E76" s="2"/>
     </row>
     <row r="77" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="70" t="s">
+      <c r="A77" s="78" t="s">
         <v>276</v>
       </c>
-      <c r="B77" s="70"/>
+      <c r="B77" s="78"/>
       <c r="C77" s="14"/>
       <c r="D77" s="14"/>
       <c r="E77" s="2"/>
     </row>
     <row r="78" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="70" t="s">
+      <c r="A78" s="78" t="s">
         <v>277</v>
       </c>
-      <c r="B78" s="70"/>
+      <c r="B78" s="78"/>
       <c r="C78" s="14"/>
       <c r="D78" s="14"/>
       <c r="E78" s="2"/>
     </row>
     <row r="79" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="70" t="s">
+      <c r="A79" s="78" t="s">
         <v>278</v>
       </c>
-      <c r="B79" s="70"/>
+      <c r="B79" s="78"/>
       <c r="C79" s="14"/>
       <c r="D79" s="14"/>
       <c r="E79" s="2"/>
     </row>
     <row r="80" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="70" t="s">
+      <c r="A80" s="78" t="s">
         <v>279</v>
       </c>
-      <c r="B80" s="70"/>
+      <c r="B80" s="78"/>
       <c r="C80" s="14"/>
       <c r="D80" s="14"/>
       <c r="E80" s="2"/>
     </row>
     <row r="81" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="70" t="s">
+      <c r="A81" s="78" t="s">
         <v>280</v>
       </c>
-      <c r="B81" s="70"/>
+      <c r="B81" s="78"/>
       <c r="C81" s="14"/>
       <c r="D81" s="14"/>
       <c r="E81" s="2"/>
     </row>
     <row r="82" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="70" t="s">
+      <c r="A82" s="78" t="s">
         <v>281</v>
       </c>
-      <c r="B82" s="70"/>
+      <c r="B82" s="78"/>
       <c r="C82" s="14"/>
       <c r="D82" s="14"/>
       <c r="E82" s="2"/>
@@ -8639,13 +8638,13 @@
       </c>
     </row>
     <row r="107" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="71" t="s">
+      <c r="A107" s="84" t="s">
         <v>353</v>
       </c>
-      <c r="B107" s="72"/>
-      <c r="C107" s="72"/>
-      <c r="D107" s="72"/>
-      <c r="E107" s="73"/>
+      <c r="B107" s="85"/>
+      <c r="C107" s="85"/>
+      <c r="D107" s="85"/>
+      <c r="E107" s="86"/>
     </row>
     <row r="108" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="17" t="s">
@@ -9009,14 +9008,14 @@
       <c r="G127" s="27"/>
     </row>
     <row r="128" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="74" t="s">
+      <c r="A128" s="81" t="s">
         <v>482</v>
       </c>
-      <c r="B128" s="75"/>
-      <c r="C128" s="75"/>
-      <c r="D128" s="75"/>
-      <c r="E128" s="75"/>
-      <c r="F128" s="76"/>
+      <c r="B128" s="82"/>
+      <c r="C128" s="82"/>
+      <c r="D128" s="82"/>
+      <c r="E128" s="82"/>
+      <c r="F128" s="83"/>
       <c r="G128" s="27"/>
     </row>
     <row r="129" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -9531,13 +9530,13 @@
       </c>
     </row>
     <row r="159" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="64" t="s">
+      <c r="A159" s="93" t="s">
         <v>554</v>
       </c>
-      <c r="B159" s="65"/>
-      <c r="C159" s="65"/>
-      <c r="D159" s="65"/>
-      <c r="E159" s="66"/>
+      <c r="B159" s="94"/>
+      <c r="C159" s="94"/>
+      <c r="D159" s="94"/>
+      <c r="E159" s="95"/>
     </row>
     <row r="160" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12" t="s">
@@ -9965,11 +9964,11 @@
       </c>
     </row>
     <row r="185" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="58"/>
-      <c r="B185" s="59"/>
-      <c r="C185" s="59"/>
-      <c r="D185" s="59"/>
-      <c r="E185" s="60"/>
+      <c r="A185" s="87"/>
+      <c r="B185" s="88"/>
+      <c r="C185" s="88"/>
+      <c r="D185" s="88"/>
+      <c r="E185" s="89"/>
     </row>
     <row r="186" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="42" t="s">
@@ -10397,13 +10396,13 @@
       </c>
     </row>
     <row r="211" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="67" t="s">
+      <c r="A211" s="96" t="s">
         <v>781</v>
       </c>
-      <c r="B211" s="68"/>
-      <c r="C211" s="68"/>
-      <c r="D211" s="68"/>
-      <c r="E211" s="69"/>
+      <c r="B211" s="97"/>
+      <c r="C211" s="97"/>
+      <c r="D211" s="97"/>
+      <c r="E211" s="98"/>
     </row>
     <row r="212" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="11" t="s">
@@ -10865,11 +10864,11 @@
       </c>
     </row>
     <row r="239" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="58"/>
-      <c r="B239" s="59"/>
-      <c r="C239" s="59"/>
-      <c r="D239" s="59"/>
-      <c r="E239" s="60"/>
+      <c r="A239" s="87"/>
+      <c r="B239" s="88"/>
+      <c r="C239" s="88"/>
+      <c r="D239" s="88"/>
+      <c r="E239" s="89"/>
     </row>
     <row r="240" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
@@ -11178,11 +11177,11 @@
       </c>
     </row>
     <row r="258" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="58"/>
-      <c r="B258" s="59"/>
-      <c r="C258" s="59"/>
-      <c r="D258" s="59"/>
-      <c r="E258" s="60"/>
+      <c r="A258" s="87"/>
+      <c r="B258" s="88"/>
+      <c r="C258" s="88"/>
+      <c r="D258" s="88"/>
+      <c r="E258" s="89"/>
     </row>
     <row r="259" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
@@ -11573,11 +11572,11 @@
       <c r="E284" s="2"/>
     </row>
     <row r="285" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A285" s="58"/>
-      <c r="B285" s="59"/>
-      <c r="C285" s="59"/>
-      <c r="D285" s="59"/>
-      <c r="E285" s="60"/>
+      <c r="A285" s="87"/>
+      <c r="B285" s="88"/>
+      <c r="C285" s="88"/>
+      <c r="D285" s="88"/>
+      <c r="E285" s="89"/>
     </row>
     <row r="286" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
@@ -12050,11 +12049,11 @@
       <c r="E315" s="2"/>
     </row>
     <row r="316" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A316" s="58"/>
-      <c r="B316" s="59"/>
-      <c r="C316" s="59"/>
-      <c r="D316" s="59"/>
-      <c r="E316" s="60"/>
+      <c r="A316" s="87"/>
+      <c r="B316" s="88"/>
+      <c r="C316" s="88"/>
+      <c r="D316" s="88"/>
+      <c r="E316" s="89"/>
     </row>
     <row r="317" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A317" s="45" t="s">
@@ -12361,11 +12360,11 @@
       </c>
     </row>
     <row r="335" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A335" s="61"/>
-      <c r="B335" s="62"/>
-      <c r="C335" s="62"/>
-      <c r="D335" s="62"/>
-      <c r="E335" s="63"/>
+      <c r="A335" s="90"/>
+      <c r="B335" s="91"/>
+      <c r="C335" s="91"/>
+      <c r="D335" s="91"/>
+      <c r="E335" s="92"/>
     </row>
     <row r="336" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A336" s="48" t="s">
@@ -13142,11 +13141,11 @@
       </c>
     </row>
     <row r="386" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A386" s="58"/>
-      <c r="B386" s="59"/>
-      <c r="C386" s="59"/>
-      <c r="D386" s="59"/>
-      <c r="E386" s="60"/>
+      <c r="A386" s="87"/>
+      <c r="B386" s="88"/>
+      <c r="C386" s="88"/>
+      <c r="D386" s="88"/>
+      <c r="E386" s="89"/>
     </row>
     <row r="387" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A387" s="5" t="s">
@@ -13519,562 +13518,562 @@
       </c>
     </row>
     <row r="409" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A409" s="86" t="s">
+      <c r="A409" s="65" t="s">
         <v>1458</v>
       </c>
-      <c r="B409" s="80" t="s">
+      <c r="B409" s="59" t="s">
         <v>1459</v>
       </c>
-      <c r="C409" s="91" t="s">
+      <c r="C409" s="70" t="s">
         <v>1460</v>
       </c>
-      <c r="D409" s="82" t="s">
+      <c r="D409" s="61" t="s">
         <v>1461</v>
       </c>
-      <c r="E409" s="81" t="s">
+      <c r="E409" s="60" t="s">
         <v>1462</v>
       </c>
     </row>
     <row r="410" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A410" s="86" t="s">
+      <c r="A410" s="65" t="s">
         <v>1463</v>
       </c>
-      <c r="B410" s="84" t="s">
+      <c r="B410" s="63" t="s">
         <v>1464</v>
       </c>
-      <c r="C410" s="92" t="s">
+      <c r="C410" s="71" t="s">
         <v>1465</v>
       </c>
-      <c r="D410" s="84" t="s">
+      <c r="D410" s="63" t="s">
         <v>1466</v>
       </c>
-      <c r="E410" s="84" t="s">
+      <c r="E410" s="63" t="s">
         <v>1467</v>
       </c>
     </row>
     <row r="411" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A411" s="89" t="s">
+      <c r="A411" s="68" t="s">
         <v>1468</v>
       </c>
-      <c r="B411" s="92" t="s">
+      <c r="B411" s="71" t="s">
         <v>1469</v>
       </c>
-      <c r="C411" s="85" t="s">
+      <c r="C411" s="64" t="s">
         <v>1470</v>
       </c>
-      <c r="D411" s="85" t="s">
+      <c r="D411" s="64" t="s">
         <v>1471</v>
       </c>
-      <c r="E411" s="85" t="s">
+      <c r="E411" s="64" t="s">
         <v>1472</v>
       </c>
     </row>
     <row r="412" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A412" s="89" t="s">
+      <c r="A412" s="68" t="s">
         <v>1473</v>
       </c>
-      <c r="B412" s="90" t="s">
+      <c r="B412" s="69" t="s">
         <v>1474</v>
       </c>
-      <c r="C412" s="90" t="s">
+      <c r="C412" s="69" t="s">
         <v>1475</v>
       </c>
-      <c r="D412" s="85" t="s">
+      <c r="D412" s="64" t="s">
         <v>666</v>
       </c>
-      <c r="E412" s="92" t="s">
+      <c r="E412" s="71" t="s">
         <v>1476</v>
       </c>
     </row>
     <row r="413" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A413" s="89" t="s">
+      <c r="A413" s="68" t="s">
         <v>1477</v>
       </c>
-      <c r="B413" s="90">
+      <c r="B413" s="69">
         <v>6</v>
       </c>
-      <c r="C413" s="90">
+      <c r="C413" s="69">
         <v>4</v>
       </c>
-      <c r="D413" s="90">
+      <c r="D413" s="69">
         <v>3</v>
       </c>
-      <c r="E413" s="92">
+      <c r="E413" s="71">
         <v>2</v>
       </c>
     </row>
     <row r="414" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A414" s="89" t="s">
+      <c r="A414" s="68" t="s">
         <v>1478</v>
       </c>
-      <c r="B414" s="84" t="s">
+      <c r="B414" s="63" t="s">
         <v>1479</v>
       </c>
-      <c r="C414" s="93" t="s">
+      <c r="C414" s="72" t="s">
         <v>1480</v>
       </c>
-      <c r="D414" s="84" t="s">
+      <c r="D414" s="63" t="s">
         <v>1481</v>
       </c>
-      <c r="E414" s="84" t="s">
+      <c r="E414" s="63" t="s">
         <v>1472</v>
       </c>
     </row>
     <row r="415" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A415" s="87"/>
-      <c r="B415" s="79"/>
-      <c r="C415" s="79"/>
-      <c r="D415" s="79"/>
-      <c r="E415" s="79"/>
+      <c r="A415" s="66"/>
+      <c r="B415" s="58"/>
+      <c r="C415" s="58"/>
+      <c r="D415" s="58"/>
+      <c r="E415" s="58"/>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E416" s="27"/>
     </row>
     <row r="417" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A417" s="89" t="s">
+      <c r="A417" s="68" t="s">
         <v>1482</v>
       </c>
-      <c r="B417" s="90" t="s">
+      <c r="B417" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="C417" s="92" t="s">
+      <c r="C417" s="71" t="s">
         <v>1483</v>
       </c>
-      <c r="D417" s="90" t="s">
+      <c r="D417" s="69" t="s">
         <v>1484</v>
       </c>
-      <c r="E417" s="90" t="s">
+      <c r="E417" s="69" t="s">
         <v>1485</v>
       </c>
     </row>
     <row r="418" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A418" s="88" t="s">
+      <c r="A418" s="67" t="s">
         <v>1486</v>
       </c>
-      <c r="B418" s="85" t="s">
+      <c r="B418" s="64" t="s">
         <v>1487</v>
       </c>
-      <c r="C418" s="85" t="s">
+      <c r="C418" s="64" t="s">
         <v>1488</v>
       </c>
-      <c r="D418" s="85" t="s">
+      <c r="D418" s="64" t="s">
         <v>1489</v>
       </c>
-      <c r="E418" s="92" t="s">
+      <c r="E418" s="71" t="s">
         <v>1490</v>
       </c>
     </row>
     <row r="419" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A419" s="84" t="s">
+      <c r="A419" s="63" t="s">
         <v>1491</v>
       </c>
-      <c r="B419" s="83" t="s">
+      <c r="B419" s="62" t="s">
         <v>1492</v>
       </c>
-      <c r="C419" s="92" t="s">
+      <c r="C419" s="71" t="s">
         <v>1493</v>
       </c>
-      <c r="D419" s="85" t="s">
+      <c r="D419" s="64" t="s">
         <v>1494</v>
       </c>
-      <c r="E419" s="90" t="s">
+      <c r="E419" s="69" t="s">
         <v>1472</v>
       </c>
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A420" s="94" t="s">
+      <c r="A420" s="73" t="s">
         <v>1495</v>
       </c>
-      <c r="B420" s="95" t="s">
+      <c r="B420" s="74" t="s">
         <v>1576</v>
       </c>
-      <c r="C420" s="94" t="s">
+      <c r="C420" s="73" t="s">
         <v>1496</v>
       </c>
-      <c r="D420" s="94" t="s">
+      <c r="D420" s="73" t="s">
         <v>1497</v>
       </c>
-      <c r="E420" s="94" t="s">
+      <c r="E420" s="73" t="s">
         <v>1498</v>
       </c>
     </row>
     <row r="421" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A421" s="94" t="s">
+      <c r="A421" s="73" t="s">
         <v>1499</v>
       </c>
-      <c r="B421" s="95" t="s">
+      <c r="B421" s="74" t="s">
         <v>1577</v>
       </c>
-      <c r="C421" s="94" t="s">
+      <c r="C421" s="73" t="s">
         <v>1500</v>
       </c>
-      <c r="D421" s="94" t="s">
+      <c r="D421" s="73" t="s">
         <v>1501</v>
       </c>
-      <c r="E421" s="94" t="s">
+      <c r="E421" s="73" t="s">
         <v>1502</v>
       </c>
     </row>
     <row r="422" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A422" s="96" t="s">
+      <c r="A422" s="75" t="s">
         <v>1503</v>
       </c>
-      <c r="B422" s="94" t="s">
+      <c r="B422" s="73" t="s">
         <v>1504</v>
       </c>
-      <c r="C422" s="94" t="s">
+      <c r="C422" s="73" t="s">
         <v>1505</v>
       </c>
-      <c r="D422" s="94" t="s">
+      <c r="D422" s="73" t="s">
         <v>1506</v>
       </c>
-      <c r="E422" s="95" t="s">
+      <c r="E422" s="74" t="s">
         <v>1578</v>
       </c>
     </row>
     <row r="423" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A423" s="94" t="s">
+      <c r="A423" s="73" t="s">
         <v>1507</v>
       </c>
-      <c r="B423" s="94" t="s">
+      <c r="B423" s="73" t="s">
         <v>1508</v>
       </c>
-      <c r="C423" s="94" t="s">
+      <c r="C423" s="73" t="s">
         <v>1509</v>
       </c>
-      <c r="D423" s="94" t="s">
+      <c r="D423" s="73" t="s">
         <v>1510</v>
       </c>
-      <c r="E423" s="95" t="s">
+      <c r="E423" s="74" t="s">
         <v>1578</v>
       </c>
     </row>
     <row r="424" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A424" s="94" t="s">
+      <c r="A424" s="73" t="s">
         <v>1511</v>
       </c>
-      <c r="B424" s="94" t="s">
+      <c r="B424" s="73" t="s">
         <v>1512</v>
       </c>
-      <c r="C424" s="95" t="s">
+      <c r="C424" s="74" t="s">
         <v>1579</v>
       </c>
-      <c r="D424" s="94" t="s">
+      <c r="D424" s="73" t="s">
         <v>1513</v>
       </c>
-      <c r="E424" s="94" t="s">
+      <c r="E424" s="73" t="s">
         <v>1514</v>
       </c>
     </row>
     <row r="425" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A425" s="94" t="s">
+      <c r="A425" s="73" t="s">
         <v>1515</v>
       </c>
-      <c r="B425" s="94" t="s">
+      <c r="B425" s="73" t="s">
         <v>1516</v>
       </c>
-      <c r="C425" s="98" t="s">
+      <c r="C425" s="77" t="s">
         <v>1517</v>
       </c>
-      <c r="D425" s="94" t="s">
+      <c r="D425" s="73" t="s">
         <v>1518</v>
       </c>
-      <c r="E425" s="94" t="s">
+      <c r="E425" s="73" t="s">
         <v>1519</v>
       </c>
     </row>
     <row r="426" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A426" s="94" t="s">
+      <c r="A426" s="73" t="s">
         <v>1520</v>
       </c>
-      <c r="B426" s="94" t="s">
+      <c r="B426" s="73" t="s">
         <v>1521</v>
       </c>
-      <c r="C426" s="94" t="s">
+      <c r="C426" s="73" t="s">
         <v>1522</v>
       </c>
-      <c r="D426" s="95" t="s">
+      <c r="D426" s="74" t="s">
         <v>1580</v>
       </c>
-      <c r="E426" s="94" t="s">
+      <c r="E426" s="73" t="s">
         <v>1519</v>
       </c>
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A427" s="94" t="s">
+      <c r="A427" s="73" t="s">
         <v>1523</v>
       </c>
-      <c r="B427" s="94" t="s">
+      <c r="B427" s="73" t="s">
         <v>1524</v>
       </c>
-      <c r="C427" s="94" t="s">
+      <c r="C427" s="73" t="s">
         <v>1525</v>
       </c>
-      <c r="D427" s="94" t="s">
+      <c r="D427" s="73" t="s">
         <v>1526</v>
       </c>
-      <c r="E427" s="95" t="s">
+      <c r="E427" s="74" t="s">
         <v>1581</v>
       </c>
     </row>
     <row r="428" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A428" s="94" t="s">
+      <c r="A428" s="73" t="s">
         <v>1527</v>
       </c>
-      <c r="B428" s="94" t="s">
+      <c r="B428" s="73" t="s">
         <v>1528</v>
       </c>
-      <c r="C428" s="94" t="s">
+      <c r="C428" s="73" t="s">
         <v>1529</v>
       </c>
-      <c r="D428" s="95" t="s">
+      <c r="D428" s="74" t="s">
         <v>1582</v>
       </c>
-      <c r="E428" s="94" t="s">
+      <c r="E428" s="73" t="s">
         <v>1530</v>
       </c>
     </row>
     <row r="429" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A429" s="94" t="s">
+      <c r="A429" s="73" t="s">
         <v>1531</v>
       </c>
-      <c r="B429" s="94" t="s">
+      <c r="B429" s="73" t="s">
         <v>1532</v>
       </c>
-      <c r="C429" s="95" t="s">
+      <c r="C429" s="74" t="s">
         <v>1583</v>
       </c>
-      <c r="D429" s="94" t="s">
+      <c r="D429" s="73" t="s">
         <v>1533</v>
       </c>
-      <c r="E429" s="94" t="s">
+      <c r="E429" s="73" t="s">
         <v>1534</v>
       </c>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A430" s="94" t="s">
+      <c r="A430" s="73" t="s">
         <v>1535</v>
       </c>
-      <c r="B430" s="94" t="s">
+      <c r="B430" s="73" t="s">
         <v>1536</v>
       </c>
-      <c r="C430" s="94" t="s">
+      <c r="C430" s="73" t="s">
         <v>1537</v>
       </c>
-      <c r="D430" s="94" t="s">
+      <c r="D430" s="73" t="s">
         <v>1538</v>
       </c>
-      <c r="E430" s="95" t="s">
+      <c r="E430" s="74" t="s">
         <v>1584</v>
       </c>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A431" s="94" t="s">
+      <c r="A431" s="73" t="s">
         <v>1539</v>
       </c>
-      <c r="B431" s="94" t="s">
+      <c r="B431" s="73" t="s">
         <v>1524</v>
       </c>
-      <c r="C431" s="94" t="s">
+      <c r="C431" s="73" t="s">
         <v>1540</v>
       </c>
-      <c r="D431" s="94" t="s">
+      <c r="D431" s="73" t="s">
         <v>1541</v>
       </c>
-      <c r="E431" s="95" t="s">
+      <c r="E431" s="74" t="s">
         <v>1585</v>
       </c>
     </row>
     <row r="432" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A432" s="94" t="s">
+      <c r="A432" s="73" t="s">
         <v>1542</v>
       </c>
-      <c r="B432" s="94" t="s">
+      <c r="B432" s="73" t="s">
         <v>1543</v>
       </c>
-      <c r="C432" s="94" t="s">
+      <c r="C432" s="73" t="s">
         <v>1537</v>
       </c>
-      <c r="D432" s="95" t="s">
+      <c r="D432" s="74" t="s">
         <v>1586</v>
       </c>
-      <c r="E432" s="94" t="s">
+      <c r="E432" s="73" t="s">
         <v>1544</v>
       </c>
     </row>
     <row r="433" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A433" s="94" t="s">
+      <c r="A433" s="73" t="s">
         <v>1545</v>
       </c>
-      <c r="B433" s="94" t="s">
+      <c r="B433" s="73" t="s">
         <v>1546</v>
       </c>
-      <c r="C433" s="94" t="s">
+      <c r="C433" s="73" t="s">
         <v>1547</v>
       </c>
-      <c r="D433" s="95" t="s">
+      <c r="D433" s="74" t="s">
         <v>1587</v>
       </c>
-      <c r="E433" s="94" t="s">
+      <c r="E433" s="73" t="s">
         <v>1548</v>
       </c>
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A434" s="94" t="s">
+      <c r="A434" s="73" t="s">
         <v>1549</v>
       </c>
-      <c r="B434" s="94" t="s">
+      <c r="B434" s="73" t="s">
         <v>1550</v>
       </c>
-      <c r="C434" s="94" t="s">
+      <c r="C434" s="73" t="s">
         <v>1551</v>
       </c>
-      <c r="D434" s="95" t="s">
+      <c r="D434" s="74" t="s">
         <v>1588</v>
       </c>
-      <c r="E434" s="94" t="s">
+      <c r="E434" s="73" t="s">
         <v>1552</v>
       </c>
     </row>
     <row r="435" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A435" s="94" t="s">
+      <c r="A435" s="73" t="s">
         <v>1553</v>
       </c>
-      <c r="B435" s="94" t="s">
+      <c r="B435" s="73" t="s">
         <v>1554</v>
       </c>
-      <c r="C435" s="95" t="s">
+      <c r="C435" s="74" t="s">
         <v>1589</v>
       </c>
-      <c r="D435" s="94" t="s">
+      <c r="D435" s="73" t="s">
         <v>1555</v>
       </c>
-      <c r="E435" s="94" t="s">
+      <c r="E435" s="73" t="s">
         <v>1556</v>
       </c>
     </row>
     <row r="436" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A436" s="94" t="s">
+      <c r="A436" s="73" t="s">
         <v>1557</v>
       </c>
-      <c r="B436" s="94" t="s">
+      <c r="B436" s="73" t="s">
         <v>1558</v>
       </c>
-      <c r="C436" s="95" t="s">
+      <c r="C436" s="74" t="s">
         <v>1590</v>
       </c>
-      <c r="D436" s="94" t="s">
+      <c r="D436" s="73" t="s">
         <v>1559</v>
       </c>
-      <c r="E436" s="94" t="s">
+      <c r="E436" s="73" t="s">
         <v>1560</v>
       </c>
     </row>
     <row r="437" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A437" s="94" t="s">
+      <c r="A437" s="73" t="s">
         <v>1561</v>
       </c>
-      <c r="B437" s="94" t="s">
+      <c r="B437" s="73" t="s">
         <v>1562</v>
       </c>
-      <c r="C437" s="94" t="s">
+      <c r="C437" s="73" t="s">
         <v>1563</v>
       </c>
-      <c r="D437" s="95" t="s">
+      <c r="D437" s="74" t="s">
         <v>1591</v>
       </c>
-      <c r="E437" s="94" t="s">
+      <c r="E437" s="73" t="s">
         <v>1519</v>
       </c>
     </row>
     <row r="438" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A438" s="94" t="s">
+      <c r="A438" s="73" t="s">
         <v>1564</v>
       </c>
-      <c r="B438" s="95" t="s">
+      <c r="B438" s="74" t="s">
         <v>1592</v>
       </c>
-      <c r="C438" s="94" t="s">
+      <c r="C438" s="73" t="s">
         <v>1547</v>
       </c>
-      <c r="D438" s="94" t="s">
+      <c r="D438" s="73" t="s">
         <v>1565</v>
       </c>
-      <c r="E438" s="94" t="s">
+      <c r="E438" s="73" t="s">
         <v>1519</v>
       </c>
     </row>
     <row r="439" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A439" s="94" t="s">
+      <c r="A439" s="73" t="s">
         <v>1566</v>
       </c>
-      <c r="B439" s="94" t="s">
+      <c r="B439" s="73" t="s">
         <v>1567</v>
       </c>
-      <c r="C439" s="95" t="s">
+      <c r="C439" s="74" t="s">
         <v>1593</v>
       </c>
-      <c r="D439" s="94" t="s">
+      <c r="D439" s="73" t="s">
         <v>1568</v>
       </c>
-      <c r="E439" s="94" t="s">
+      <c r="E439" s="73" t="s">
         <v>1502</v>
       </c>
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A440" s="94" t="s">
+      <c r="A440" s="73" t="s">
         <v>1569</v>
       </c>
-      <c r="B440" s="95" t="s">
+      <c r="B440" s="74" t="s">
         <v>1594</v>
       </c>
-      <c r="C440" s="94" t="s">
+      <c r="C440" s="73" t="s">
         <v>1570</v>
       </c>
-      <c r="D440" s="94" t="s">
+      <c r="D440" s="73" t="s">
         <v>1571</v>
       </c>
-      <c r="E440" s="94" t="s">
+      <c r="E440" s="73" t="s">
         <v>1572</v>
       </c>
     </row>
     <row r="441" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A441" s="94" t="s">
+      <c r="A441" s="73" t="s">
         <v>1573</v>
       </c>
-      <c r="B441" s="94" t="s">
+      <c r="B441" s="73" t="s">
         <v>1574</v>
       </c>
-      <c r="C441" s="95" t="s">
+      <c r="C441" s="74" t="s">
         <v>1595</v>
       </c>
-      <c r="D441" s="97" t="s">
+      <c r="D441" s="76" t="s">
         <v>1575</v>
       </c>
-      <c r="E441" s="94" t="s">
+      <c r="E441" s="73" t="s">
         <v>1502</v>
       </c>
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A442" s="94"/>
-      <c r="B442" s="94"/>
-      <c r="C442" s="94"/>
-      <c r="D442" s="94"/>
-      <c r="E442" s="94"/>
+      <c r="A442" s="73"/>
+      <c r="B442" s="73"/>
+      <c r="C442" s="73"/>
+      <c r="D442" s="73"/>
+      <c r="E442" s="73"/>
     </row>
     <row r="443" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A443" s="94"/>
-      <c r="B443" s="94"/>
-      <c r="C443" s="94"/>
-      <c r="D443" s="94"/>
-      <c r="E443" s="94"/>
+      <c r="A443" s="73"/>
+      <c r="B443" s="73"/>
+      <c r="C443" s="73"/>
+      <c r="D443" s="73"/>
+      <c r="E443" s="73"/>
     </row>
     <row r="444" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A444" s="94"/>
-      <c r="B444" s="94"/>
-      <c r="C444" s="94"/>
-      <c r="D444" s="94"/>
-      <c r="E444" s="94"/>
+      <c r="A444" s="73"/>
+      <c r="B444" s="73"/>
+      <c r="C444" s="73"/>
+      <c r="D444" s="73"/>
+      <c r="E444" s="73"/>
     </row>
     <row r="445" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E445" s="27"/>
@@ -14630,12 +14629,15 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A316:E316"/>
+    <mergeCell ref="A335:E335"/>
+    <mergeCell ref="A386:E386"/>
+    <mergeCell ref="A159:E159"/>
+    <mergeCell ref="A185:E185"/>
+    <mergeCell ref="A211:E211"/>
+    <mergeCell ref="A239:E239"/>
+    <mergeCell ref="A258:E258"/>
+    <mergeCell ref="A285:E285"/>
     <mergeCell ref="A128:F128"/>
     <mergeCell ref="A73:B73"/>
     <mergeCell ref="A74:B74"/>
@@ -14648,24 +14650,21 @@
     <mergeCell ref="A81:B81"/>
     <mergeCell ref="A82:B82"/>
     <mergeCell ref="A107:E107"/>
-    <mergeCell ref="A316:E316"/>
-    <mergeCell ref="A335:E335"/>
-    <mergeCell ref="A386:E386"/>
-    <mergeCell ref="A159:E159"/>
-    <mergeCell ref="A185:E185"/>
-    <mergeCell ref="A211:E211"/>
-    <mergeCell ref="A239:E239"/>
-    <mergeCell ref="A258:E258"/>
-    <mergeCell ref="A285:E285"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B48" r:id="rId1" display=".@using" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B92" r:id="rId2" display="a.@Html.Editor" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A93" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A94" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A91" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B48" r:id="rId1" display=".@using"/>
+    <hyperlink ref="B92" r:id="rId2" display="a.@Html.Editor"/>
+    <hyperlink ref="A93" r:id="rId3"/>
+    <hyperlink ref="A94" r:id="rId4"/>
+    <hyperlink ref="A91" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <pageSetup paperSize="3" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>